<commit_message>
added feed till september
</commit_message>
<xml_diff>
--- a/DataFeeds/FoodPriceIndex_FAO.xlsx
+++ b/DataFeeds/FoodPriceIndex_FAO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBFD871-375F-47E7-BE02-A1BEBE447F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63BFF85-AD47-4530-AEDF-4737B03A4D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B2DA42F1-6EA0-4C56-BA21-E21AAE3FA26C}"/>
+    <workbookView xWindow="28690" yWindow="2460" windowWidth="24220" windowHeight="13120" xr2:uid="{B2DA42F1-6EA0-4C56-BA21-E21AAE3FA26C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>2022 08</t>
+  </si>
+  <si>
+    <t>2022 09</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F37AE00-0E9B-4B95-9B55-969227118D25}">
-  <dimension ref="A1:B393"/>
+  <dimension ref="A1:B394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="D389" sqref="D389"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="A393" sqref="A393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3635,6 +3638,14 @@
         <v>138</v>
       </c>
     </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B394" s="5">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>